<commit_message>
Automatische test-sync: 2025-06-26 18:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -65,7 +65,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -98,6 +98,13 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="00D9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFF2CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -211,12 +218,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +653,11 @@
           <t>Beantwoord</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Handmatig opvolgen</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -689,8 +701,62 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kunnen jullie ook maatwerk leveren voor beurzen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Goedemiddag, 
+Wij zijn op zoek naar maatwerk displays voor een beurs in september. Kunnen jullie dit soort werk leveren, en zo ja, wat zijn de mogelijkheden en levertijden?
+Alvast bedankt!
+Met vriendelijke groet, 
+M. Peters
+Marketing &amp; Events
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste M. Peters,
+Hartelijk dank voor uw interesse in maatwerk displays voor uw beurs in september. Ja, wij kunnen zeker maatwerk displays leveren. Om u goed te kunnen helpen, ontvangen we graag meer informatie over uw specifieke wensen en eisen voor de displays. Hierdoor kunnen we u voorzien van de best passende opties en bijbehorende levertijden.
+Kunt u meer details geven over de gewenste afmetingen, materialen, eventuele speciale functies, en de hoeveelheid displays die u nodig heeft? Met deze informatie kunnen we een passende offerte op maat voor u opstellen en uitleggen wat de mogelijkheden zijn.
+Indien u ons meer details kunt verstrekken, kunnen we samen verder kijken naar de beste oplossing voor uw beurs in september.
+Met vriendelijke groet,
+[Bedrijfsnaam] 
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-26 18:47:57</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -710,12 +776,17 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="0">
       <formula>"Nee"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H3">
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
+      <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -728,7 +799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -758,6 +829,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 18:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -609,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,8 +755,62 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kan ik een offerte krijgen voor maatwerk wandkasten met ingebouwde
+ koeling?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Goedemiddag, 
+Wij zijn op zoek naar op maat gemaakte wandkasten met geïntegreerde koeling voor een farmaceutische toepassing. Kunt u hiervoor een offerte maken en uitleggen wat de technische mogelijkheden zijn?
+Met vriendelijke groet, 
+L. Kruger 
+Medicorp GmbH
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Geachte heer Kruger,
+Hartelijk dank voor uw interesse in onze op maat gemaakte wandkasten met geïntegreerde koeling voor farmaceutische toepassingen. Wij stellen graag een offerte voor u op en zullen uitleggen welke technische mogelijkheden beschikbaar zijn.
+Voor een accurate offerte en om de technische mogelijkheden toe te lichten, zouden we graag meer details willen ontvangen over uw specifieke wensen en vereisten. Kunt u ons informatie verschaffen over de gewenste afmetingen, specifieke koelvereisten en eventuele andere functionaliteiten die belangrijk zijn voor uw toepassing?
+Zodra wij deze informatie hebben ontvangen, zullen wij snel een gedetailleerde offerte opstellen en de technische mogelijkheden met u bespreken.
+Met vriendelijke groet,
+[Je Naam]
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-26 18:52:16</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -776,7 +830,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -784,7 +838,7 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +876,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 18:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -218,12 +218,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -609,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,8 +809,58 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tvvccxx hghhgg rtrtrt. Kan dit?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Hallo, 
+Tvvccxx hghhgg rtrtrt blabla. Is dit mogelijk op basis van de 7e afmeting van jullie multitemperatuur?
+Dank en groet 
+Jan
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste Jan,
+Bedankt voor je e-mail. Helaas begrijp ik niet helemaal wat je bedoelt met "Tvvccxx hghhgg rtrtrt blabla" en "7e afmeting van jullie multitemperatuur". Zou je meer details kunnen geven of specifieker kunnen zijn over je vraag?
+Als je nog steeds hulp nodig hebt, laat het me dan alsjeblieft weten. 
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-26 18:54:36</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -830,7 +880,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -838,7 +888,7 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
@@ -853,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,6 +943,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 18:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -218,12 +218,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -609,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,8 +859,57 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Boutjes M6x12</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>He Johan,
+Zou je voor mij M6x12 3000 stuks kunnen bestellen?
+Met vriendelijke groet,
+Marco
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste Marco,
+Bedankt voor je bericht. Helaas kan ik geen bestellingen plaatsen via e-mail. Je kunt een bestelling plaatsen via ons bestelsysteem op onze website of neem contact op met onze verkoopafdeling voor verdere assistentie.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-26 18:57:25</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -880,7 +929,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -888,7 +937,7 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
@@ -903,7 +952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,6 +1002,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -609,7 +609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,8 +908,59 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kan je voor mij 2500 M8 slotbouten bestellen bij Van Ommeren?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hoi, 
+Kun jij 2500 stuks M8 slotbouten bestellen bij Van Ommeren voor levering op donderdag? 
+Laat me weten als dit gelukt is.
+Groeten, 
+Jeroen
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste Jeroen,
+Bedankt voor je bericht. Ik ben een geautomatiseerde assistent en kan geen bestellingen plaatsen. Je kunt rechtstreeks contact opnemen met Van Ommeren om je bestelling van 2500 stuks M8 slotbouten te plaatsen voor levering op donderdag.
+Voor verdere assistentie kun je mij altijd contacteren.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:07:34</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -929,7 +980,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -937,7 +988,7 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
@@ -985,17 +1036,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1005,7 +1056,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -65,7 +65,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -105,6 +105,13 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="00FFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00C9DAF8"/>
         </patternFill>
       </fill>
     </dxf>
@@ -609,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,6 +665,11 @@
           <t>Handmatig opvolgen</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Automatisch afgehandeld</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -959,8 +971,62 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Svp 10 liter koelvloeistof bestellen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hoi, 
+Wil je voor de werkplaats 10 liter koelvloeistof bestellen? 
+Dank!
+– Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste Rick,
+Bedankt voor je e-mail. Ik ga direct 10 liter koelvloeistof voor de werkplaats bestellen. Heb je een specifiek merk of type koelvloeistof dat we moeten aanschaffen, of kan ik zelf een keuze maken?
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:20:19</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -980,7 +1046,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -988,8 +1054,13 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
+      <formula>"Ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I8">
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1026,17 +1097,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,8 +1025,61 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bestel je 3 rollen ducttape?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>He Johan,
+Zou je 3 rollen ducttape kunnen bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste Marc,
+Bedankt voor je verzoek. Ik zal direct 3 rollen ducttape bestellen. Heb je een specifieke voorkeur voor het merk of kleur? Laat het me weten, zodat ik de bestelling nauwkeurig kan plaatsen.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:26:42</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1046,7 +1099,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1054,12 +1107,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1101,7 +1154,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,8 +1078,62 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bestel je 5 paar werkhandschoenen voor me</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>He Johan
+zou je 5 paar werkhandschoenen voor mij kunnen bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste Marc,
+Bedankt voor je e-mail. Natuurlijk kan ik 5 paar werkhandschoenen voor je bestellen. Kun je me wat meer details geven, zoals het type werkhandschoenen en de maat die je nodig hebt? Als je specifieke voorkeuren hebt, laat het me dan weten zodat ik de bestelling correct kan plaatsen.
+Alvast bedankt!
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:30:33</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1099,7 +1153,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1107,12 +1161,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1154,7 +1208,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1132,8 +1132,62 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kun je 2 dozen nitrilhandschoenen bestellen?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>He Johan,
+Kun je 2 dozen nitrilhandschoenen bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Beste Marc,
+Bedankt voor je e-mail. Om je verzoek voor het bestellen van 2 dozen nitrilhandschoenen te verwerken, heb ik wat meer informatie nodig. Kun je mij laten weten welke maat(en) nitrilhandschoenen je nodig hebt? Zodra ik deze informatie van je heb ontvangen, zal ik de bestelling voor je plaatsen.
+Met vriendelijke groet,
+Johan  
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:33:20</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1153,7 +1207,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1161,12 +1215,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1208,7 +1262,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 19:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1186,8 +1186,58 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kun je 2 dozen nitrilhandschoenen bestellen?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>He Johan,
+Kun je 2 dozen nitrilhandschoenen bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-26 19:37:15</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1207,7 +1257,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1215,12 +1265,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1262,7 +1312,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 20:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1236,8 +1236,61 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wil je 4 rollen plasticfolie bestellen?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Hoi Johan,
+Wil je 4 rollen plasticfolie bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste Marc,
+Bedankt voor je e-mail. Helaas kunnen we geen bestellingen via e-mail verwerken. Je kunt eenvoudig via onze website 4 rollen plasticfolie bestellen. Mocht je hulp nodig hebben of vragen hebben over het bestelproces, dan helpen we je graag verder.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-26 20:54:55</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1257,7 +1310,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1265,12 +1318,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1312,7 +1365,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1289,8 +1289,61 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kun jij 5 pakken A4-papier bestellen?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Hoi Johan
+Kun jij 5 pakken A4-papier bestellen?
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Beste Marc,
+Bedankt voor je e-mail. Ik zorg ervoor dat er 5 pakken A4-papier worden besteld. Heb je nog specifieke voorkeuren voor het merk of type papier? Laat het me weten als je nog andere vragen hebt.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:03:25</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1310,7 +1363,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1318,12 +1371,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1365,7 +1418,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1342,8 +1342,60 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hoi Johan, 
+Zou je 10 dozen schroeven kunnen bestellen voor de werkplaats? 
+We hebben vooral maat 4x40 nodig.
+Groet, 
+Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:06:46</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1363,7 +1415,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1371,12 +1423,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1418,7 +1470,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1394,8 +1394,60 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kun je 4 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Hoi Johan, 
+Zou je 4 dozen schroeven kunnen bestellen voor de werkplaats?
+Dank je wel!
+Groet, 
+Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:11:46</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1415,7 +1467,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1423,12 +1475,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1470,7 +1522,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1446,8 +1446,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Kun je 5 liter koelvloeistof bestellen?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Hoi Johan,
+ Zou je 5 liter koelvloeistof kunnen bestellen voor de werkplaats?
+ Laat me even weten of dit lukt.
+Groet,
+ Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:16:24</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1467,7 +1519,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1475,12 +1527,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1522,7 +1574,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1498,8 +1498,61 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wil je 5 boren bestellen?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Hoi Johan,
+Wil je 5 boren bestellen?
+Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Beste Rick,
+Bedankt voor je e-mail. Om de bestelling van de 5 boren te verwerken, hebben we wat meer informatie nodig. Zou je het artikelnummer of de specifieke kenmerken van de boren kunnen doorgeven? Op die manier kunnen we ervoor zorgen dat we de juiste producten voor je bestellen.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:21:18</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1519,7 +1572,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1527,12 +1580,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1574,7 +1627,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1551,8 +1551,62 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kun je 5 rollen afplaktape bestellen?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hoi Johan,
+ Zou je 5 rollen afplaktape kunnen bestellen voor de schildersafdeling?
+Dank je wel!
+ — Marco
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste Marco,
+Bedankt voor je e-mail. We zullen direct 5 rollen afplaktape bestellen voor de schildersafdeling. Zodra de bestelling is geplaatst, ontvang je hier een bevestiging van.
+Met vriendelijke groet,
+Johan</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:25:07</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1572,7 +1626,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1580,12 +1634,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1627,7 +1681,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1605,8 +1605,60 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Kan je 500 liter antivries bestellen?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hoi Johan, 
+Zou je 500 liter antivries kunnen bestellen voor de wintervoorraad?
+Dank je wel!
+Groeten, 
+Marc 
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:29:25</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1626,7 +1678,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1634,12 +1686,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1681,7 +1733,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1657,8 +1657,59 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bestel je 3 bussen siliconenspray?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>He Johan, 
+Zou je 3 bussen siliconenspray kunnen bestellen voor in de werkplaats?
+Thanks,
+Marc
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:42:06</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1678,7 +1729,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1686,12 +1737,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1733,7 +1784,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 21:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1708,8 +1708,60 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wil je 6 dozen werkhandschoenen bestellen?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MailMind Test &lt;mailmind.test@zohomail.eu&gt;</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Hoi Johan, 
+Zou je 6 dozen werkhandschoenen kunnen bestellen voor in het magazijn? 
+We gebruiken meestal maat L.
+Groet, 
+Rick
+Sent using {0}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Bedankt voor je bericht. Ik neem dit z.s.m. in behandeling.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-26 21:51:51</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1729,7 +1781,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1737,12 +1789,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1784,7 +1836,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1760,8 +1760,58 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:15:54</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1781,7 +1831,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1789,12 +1839,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1809,7 +1859,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1869,6 +1919,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1810,8 +1810,58 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:22:21</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1831,7 +1881,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1839,12 +1889,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1892,7 +1942,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1902,17 +1952,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1922,7 +1972,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1860,8 +1860,59 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank u voor uw interesse in onze producten/diensten. Om u nauwkeurige informatie te verstrekken over de verzendkosten, hebben we meer details nodig zoals het product/dienst waar u naar informeert en het afleveradres. Zou u ons kunnen voorzien van deze informatie zodat we u een precieze schatting van de verzendkosten kunnen geven?
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:24:51</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1881,7 +1932,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1889,12 +1940,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1942,7 +1993,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1962,17 +2013,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1911,8 +1911,58 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:26:13</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1932,7 +1982,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1940,12 +1990,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1993,17 +2043,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2013,7 +2063,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1961,8 +1961,58 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:35:27</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1982,7 +2032,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1990,12 +2040,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2047,7 +2097,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2011,8 +2011,50 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:54:55</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2032,7 +2074,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2040,12 +2082,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2097,7 +2139,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 22:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2053,8 +2053,50 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-26 22:57:10</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2074,7 +2116,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2082,12 +2124,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2139,7 +2181,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2095,8 +2095,58 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:01:23</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2116,7 +2166,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2124,12 +2174,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2181,7 +2231,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2145,8 +2145,58 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:03:24</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2166,7 +2216,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2174,12 +2224,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2231,7 +2281,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2195,8 +2195,58 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:08:37</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2216,7 +2266,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2224,12 +2274,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
+  <conditionalFormatting sqref="H2:H32">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I31">
+  <conditionalFormatting sqref="I2:I32">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2281,7 +2331,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2245,8 +2245,58 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:10:55</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2266,7 +2316,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2274,12 +2324,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H32">
+  <conditionalFormatting sqref="H2:H33">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I32">
+  <conditionalFormatting sqref="I2:I33">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2331,7 +2381,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2295,8 +2295,59 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Testmail #2: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank u voor uw interesse in onze producten/diensten. Om u nauwkeurige informatie te verstrekken over de verzendkosten, hebben we meer details nodig zoals het product/dienst waar u naar informeert en het afleveradres. Zou u ons kunnen voorzien van deze informatie zodat we u een precieze schatting van de verzendkosten kunnen geven?
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:13:07</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2316,7 +2367,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2324,12 +2375,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
+  <conditionalFormatting sqref="H2:H34">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
+  <conditionalFormatting sqref="I2:I34">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2391,7 +2442,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,8 +2346,58 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Testmail #3: Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw bestelling te annuleren, hebben we wat extra informatie nodig. Zou u zo vriendelijk willen zijn om uw bestelnummer met ons te delen? Op die manier kunnen we uw verzoek snel verwerken.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:15:26</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2367,7 +2417,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2375,12 +2425,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
+  <conditionalFormatting sqref="H2:H35">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I34">
+  <conditionalFormatting sqref="I2:I35">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2448,7 +2498,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2458,11 +2508,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,8 +2396,59 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Hoe kan ik iets retourneren?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Testmail #4: Hoe kan ik iets retourneren?</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Als je een artikel wilt retourneren, kun je dit doen door contact op te nemen met onze klantenservice via support@bedrijf.nl. Zij zullen je verder begeleiden bij het retourproces en eventuele vragen beantwoorden.
+Bedankt voor je begrip en medewerking.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:17:40</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2417,7 +2468,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2425,12 +2476,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H35">
+  <conditionalFormatting sqref="H2:H36">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I35">
+  <conditionalFormatting sqref="I2:I36">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2488,7 +2539,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2498,11 +2549,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2447,8 +2447,58 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie voorwaarden?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Testmail #5: Wat zijn jullie voorwaarden?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse in onze diensten. Voor informatie over onze voorwaarden kunt u terecht op onze website onder de sectie 'Algemene Voorwaarden'. Mocht u specifieke vragen hebben, dan helpen wij u graag verder. Aarzel niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:19:51</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2468,7 +2518,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2476,12 +2526,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H36">
+  <conditionalFormatting sqref="H2:H37">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I36">
+  <conditionalFormatting sqref="I2:I37">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2539,17 +2589,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2497,8 +2497,59 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Ik heb geen orderbevestiging gekregen</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Testmail #6: Ik heb geen orderbevestiging gekregen</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om u beter van dienst te kunnen zijn, zou u ons uw bestelnummer of de datum van uw bestelling kunnen doorgeven? Hiermee kunnen we nagaan wat er mogelijk is misgegaan met de orderbevestiging.
+We doen ons best om dit zo snel mogelijk voor u op te lossen. Alvast bedankt voor uw medewerking!
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:22:07</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2518,7 +2569,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2526,12 +2577,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H37">
+  <conditionalFormatting sqref="H2:H38">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I37">
+  <conditionalFormatting sqref="I2:I38">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2573,7 +2624,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2548,8 +2548,58 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Zijn jullie telefonisch bereikbaar?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Testmail #7: Zijn jullie telefonisch bereikbaar?</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Op dit moment zijn wij helaas niet telefonisch bereikbaar. Als u vragen heeft of hulp nodig heeft, kunt u ons altijd per e-mail bereiken op dit adres. We streven ernaar om binnen 24 uur te reageren op alle vragen en verzoeken die we ontvangen.
+Met vriendelijke groet,
+[Naam van het bedrijf] assistent</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:24:20</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2569,7 +2619,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2577,12 +2627,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H38">
+  <conditionalFormatting sqref="H2:H39">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I38">
+  <conditionalFormatting sqref="I2:I39">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2634,7 +2684,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2598,8 +2598,59 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Ik wil mijn gegevens aanpassen</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Testmail #8: Ik wil mijn gegevens aanpassen</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw bericht. Om uw gegevens aan te passen, kunt u inloggen op onze website met uw gebruikersnaam en wachtwoord. Eenmaal ingelogd, kunt u uw persoonlijke gegevens bijwerken onder uw accountinstellingen.
+Mocht u nog verdere assistentie nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:26:33</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2619,7 +2670,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2627,12 +2678,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H39">
+  <conditionalFormatting sqref="H2:H40">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I39">
+  <conditionalFormatting sqref="I2:I40">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2647,7 +2698,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2717,6 +2768,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:28:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2649,8 +2649,59 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ik heb een klacht</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Testmail #9: Ik heb een klacht</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het doorsturen van uw klacht. Om uw klacht zo goed mogelijk te kunnen behandelen, ontvangen wij graag meer informatie over de aard van de klacht. Kunt u ons meer details geven over wat er precies is misgegaan? 
+Met vriendelijke groet,
+[Naam] 
+Klantenservice Team</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:28:44</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2670,7 +2721,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2678,12 +2729,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H40">
+  <conditionalFormatting sqref="H2:H41">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I40">
+  <conditionalFormatting sqref="I2:I41">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2698,7 +2749,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2778,6 +2829,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2700,8 +2700,58 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Zijn er vacatures?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Testmail #10: Zijn er vacatures?</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Beste,
+Dank u voor uw interesse in onze organisatie. Op dit moment hebben we geen openstaande vacatures, maar we moedigen u aan om regelmatig onze website te bezoeken voor eventuele toekomstige mogelijkheden. Mocht u nog vragen hebben of meer informatie wensen, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:30:58</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2721,7 +2771,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2729,12 +2779,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H41">
+  <conditionalFormatting sqref="H2:H42">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I41">
+  <conditionalFormatting sqref="I2:I42">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2749,7 +2799,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2839,6 +2889,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2750,8 +2750,60 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Testmail #11: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:33:11</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2771,7 +2823,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2779,12 +2831,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42">
+  <conditionalFormatting sqref="H2:H43">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I42">
+  <conditionalFormatting sqref="I2:I43">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2826,7 +2878,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2802,8 +2802,59 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Testmail #12: Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je interesse in ons artikel. Helaas kan ik je op basis van dit bericht niet verder helpen. Kun je meer details geven over welk artikel je wilt inkopen en op welke manier? Zo kan ik je beter assisteren.
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:45:03</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2823,7 +2874,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2831,12 +2882,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H43">
+  <conditionalFormatting sqref="H2:H44">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I43">
+  <conditionalFormatting sqref="I2:I44">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2878,7 +2929,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2853,8 +2853,59 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Testmail #13: Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Kun je wat meer specifieke informatie geven over waarover je precies wilt dat er intern overlegd wordt? Op die manier kan ik ervoor zorgen dat je aanvraag bij de juiste persoon of afdeling terechtkomt.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:47:16</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2874,7 +2925,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2882,12 +2933,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H44">
+  <conditionalFormatting sqref="H2:H45">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I44">
+  <conditionalFormatting sqref="I2:I45">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2979,7 +3030,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2904,8 +2904,58 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Kun je contact opnemen met de klant?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Testmail #14: Kun je contact opnemen met de klant?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Beste klantenservice,
+Ik heb zojuist een testmail verstuurd (Testmail #14) om te controleren of onze klanten goed bereikbaar zijn via e-mail. Kun je bevestigen of deze testmail succesvol is ontvangen en of jullie contact hebben opgenomen met de klant?
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:49:29</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2925,7 +2975,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2933,12 +2983,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H45">
+  <conditionalFormatting sqref="H2:H46">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I45">
+  <conditionalFormatting sqref="I2:I46">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3000,7 +3050,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2954,8 +2954,60 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Ik wil dat je dit regelt met support.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Testmail #15: Ik wil dat je dit regelt met support.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om uw verzoek efficiënt te kunnen afhandelen, zou ik graag wat meer informatie van u willen ontvangen. Kunt u mij alstublieft meer details geven over het specifieke probleem waarmee u hulp nodig heeft? Op die manier kunnen wij u beter van dienst zijn.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent  
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:51:43</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2975,7 +3027,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2983,12 +3035,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H46">
+  <conditionalFormatting sqref="H2:H47">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I46">
+  <conditionalFormatting sqref="I2:I47">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3066,17 +3118,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3006,8 +3006,58 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Wanneer komt mijn offerte?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Testmail #16: Wanneer komt mijn offerte?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw e-mail. Uw offerte zal naar verwachting binnen 24 uur worden verstuurd. Mocht u deze niet op tijd ontvangen, neem dan gerust contact met ons op.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:53:56</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D47">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3027,7 +3077,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G47">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3035,12 +3085,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H47">
+  <conditionalFormatting sqref="H2:H48">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I47">
+  <conditionalFormatting sqref="I2:I48">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3108,7 +3158,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3118,7 +3168,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -3128,11 +3178,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3056,8 +3056,58 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Kun je deze bestelling vandaag verwerken?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Testmail #17: Kun je deze bestelling vandaag verwerken?</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw e-mail. Om de bestelling vandaag te kunnen verwerken, hebben we een ordernummer of klantgegevens nodig. Zou u ons deze gegevens kunnen verstrekken, zodat we uw verzoek verder kunnen onderzoeken?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:56:10</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3077,7 +3127,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3085,12 +3135,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H48">
+  <conditionalFormatting sqref="H2:H49">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I48">
+  <conditionalFormatting sqref="I2:I49">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3132,7 +3182,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-26 23:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-26.xlsx
+++ b/logs/mail_log_2025-06-26.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3106,8 +3106,58 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Kun je dit product voor mij bestellen?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Testmail #18: Kun je dit product voor mij bestellen?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u wel voor uw interesse in ons product. Helaas kunnen wij op basis van deze e-mail geen bestelling voor u plaatsen. U kunt echter onze website bezoeken en het product zelf bestellen. Mocht u verdere vragen hebben of hulp nodig hebben bij het plaatsen van een bestelling, dan helpen wij u graag verder.
+Met vriendelijke groet,
+[Naam Bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-06-26 23:58:23</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -3127,7 +3177,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3135,12 +3185,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H49">
+  <conditionalFormatting sqref="H2:H50">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I49">
+  <conditionalFormatting sqref="I2:I50">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -3182,7 +3232,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">

</xml_diff>